<commit_message>
extended ip-plan and added some interfaces
</commit_message>
<xml_diff>
--- a/data/documentation.xlsx
+++ b/data/documentation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
   </bookViews>
   <sheets>
     <sheet name="IP-plan" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="133">
   <si>
     <t>IP-address</t>
   </si>
@@ -128,9 +128,6 @@
     <t>192.4.2.1</t>
   </si>
   <si>
-    <t>192.4.2.2 - 192.4.2.254</t>
-  </si>
-  <si>
     <t>192.4.3.0/24</t>
   </si>
   <si>
@@ -272,9 +269,6 @@
     <t>FE 0/19 - FE 0/22</t>
   </si>
   <si>
-    <t>UpLink</t>
-  </si>
-  <si>
     <t>2,3,101,102,103,104</t>
   </si>
   <si>
@@ -318,6 +312,120 @@
   </si>
   <si>
     <t>Printers</t>
+  </si>
+  <si>
+    <t>Moscow</t>
+  </si>
+  <si>
+    <t>192.4.0.0/20</t>
+  </si>
+  <si>
+    <t>Saint-Petersburg</t>
+  </si>
+  <si>
+    <t>192.4.16.0/21</t>
+  </si>
+  <si>
+    <t>Kemerovo</t>
+  </si>
+  <si>
+    <t>192.4.24.0/22</t>
+  </si>
+  <si>
+    <t>192.4.16.1</t>
+  </si>
+  <si>
+    <t>spb-vsl-gw1</t>
+  </si>
+  <si>
+    <t>spb-vsl-dsw1</t>
+  </si>
+  <si>
+    <t>192.4.16.2</t>
+  </si>
+  <si>
+    <t>192.4.16.0/24</t>
+  </si>
+  <si>
+    <t>Vsl. Ostrov</t>
+  </si>
+  <si>
+    <t>192.4.16.25 - 192.4.16.254</t>
+  </si>
+  <si>
+    <t>192.4.17.0/24</t>
+  </si>
+  <si>
+    <t>Ozerki</t>
+  </si>
+  <si>
+    <t>spb-ozerki-gw1</t>
+  </si>
+  <si>
+    <t>192.4.17.1</t>
+  </si>
+  <si>
+    <t>192.4.17.25 - 192.4.17.254</t>
+  </si>
+  <si>
+    <t>Krasnaya Gorka</t>
+  </si>
+  <si>
+    <t>192.4.24.0/24</t>
+  </si>
+  <si>
+    <t>kmr-gorka-gw1</t>
+  </si>
+  <si>
+    <t>kmr-gorka-dsw1</t>
+  </si>
+  <si>
+    <t>192.4.24.1</t>
+  </si>
+  <si>
+    <t>192.4.24.2</t>
+  </si>
+  <si>
+    <t>192.4.24.25 - 192.4.24.254</t>
+  </si>
+  <si>
+    <t>192.4.2.2</t>
+  </si>
+  <si>
+    <t>192.4.2.0/28</t>
+  </si>
+  <si>
+    <t>192.4.2.0/30</t>
+  </si>
+  <si>
+    <t>192.4.2.4/30</t>
+  </si>
+  <si>
+    <t>192.4.2.5</t>
+  </si>
+  <si>
+    <t>192.4.2.6</t>
+  </si>
+  <si>
+    <t>192.4.2.8 - 192.4.2.15</t>
+  </si>
+  <si>
+    <t>192.4.2.16/30</t>
+  </si>
+  <si>
+    <t>192.4.2.20 - 192.4.2.254</t>
+  </si>
+  <si>
+    <t>192.4.2.17</t>
+  </si>
+  <si>
+    <t>192.4.2.18</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>FILL</t>
   </si>
 </sst>
 </file>
@@ -359,12 +467,18 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -379,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -395,6 +509,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -676,15 +812,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -704,282 +840,521 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C5" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2</v>
-      </c>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="3"/>
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>31</v>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
       </c>
       <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="3"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="8"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="3">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="3">
-        <v>102</v>
-      </c>
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>120</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" t="s">
-        <v>36</v>
+    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="3">
-        <v>103</v>
-      </c>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" t="s">
-        <v>11</v>
+      <c r="A27" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" t="s">
-        <v>36</v>
+      <c r="A28" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="10"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="10"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="10"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="3"/>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="3">
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="9"/>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="3"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="3"/>
+      <c r="B50" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C56" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>119</v>
+      </c>
+      <c r="B60" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1004,10 +1379,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1018,10 +1393,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1032,7 +1407,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1043,12 +1418,12 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -1060,10 +1435,10 @@
         <v>101</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1071,10 +1446,10 @@
         <v>102</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1082,10 +1457,10 @@
         <v>103</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1093,10 +1468,10 @@
         <v>104</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1106,10 +1481,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,189 +1498,177 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="C5" s="4" t="s">
-        <v>26</v>
+        <v>131</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="4">
-        <v>2.2999999999999998</v>
-      </c>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
-        <v>83</v>
-      </c>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="A7" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="B7" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4">
+        <v>2.2999999999999998</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="4">
-        <v>2.2999999999999998</v>
+      <c r="E9" s="4" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="4">
-        <v>2.2999999999999998</v>
+      <c r="E10" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="4">
-        <v>3</v>
-      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+      <c r="A12" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="B12" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D12" s="4">
-        <v>3</v>
-      </c>
-      <c r="E12" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4">
+        <v>2.2999999999999998</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="E13" s="4">
+        <v>2.2999999999999998</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4">
-        <v>2.2999999999999998</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="D14" s="4">
+        <v>3</v>
+      </c>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D15" s="4">
         <v>3</v>
@@ -1321,127 +1684,439 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D17" s="4"/>
-      <c r="E17" s="4" t="s">
-        <v>83</v>
+      <c r="E17" s="4">
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="D18" s="4">
-        <v>101</v>
+        <v>3</v>
       </c>
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="4">
-        <v>102</v>
-      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="A20" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B20" s="4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="4">
-        <v>103</v>
-      </c>
-      <c r="E20" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="D21" s="4">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="B22" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="4">
+        <v>102</v>
+      </c>
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="A23" s="4"/>
       <c r="B23" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4" t="s">
-        <v>84</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D23" s="4">
+        <v>103</v>
+      </c>
+      <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D24" s="4">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D25" s="4">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="4">
+        <v>101</v>
+      </c>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="4">
         <v>104</v>
       </c>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="13">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E33" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E34" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>132</v>
+      </c>
+      <c r="B41" t="s">
+        <v>132</v>
+      </c>
+      <c r="C41" t="s">
+        <v>132</v>
+      </c>
+      <c r="D41" t="s">
+        <v>132</v>
+      </c>
+      <c r="E41" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>132</v>
+      </c>
+      <c r="B42" t="s">
+        <v>132</v>
+      </c>
+      <c r="C42" t="s">
+        <v>132</v>
+      </c>
+      <c r="D42" t="s">
+        <v>132</v>
+      </c>
+      <c r="E42" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>132</v>
+      </c>
+      <c r="B43" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" t="s">
+        <v>132</v>
+      </c>
+      <c r="D43" t="s">
+        <v>132</v>
+      </c>
+      <c r="E43" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>132</v>
+      </c>
+      <c r="B44" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" t="s">
+        <v>132</v>
+      </c>
+      <c r="D44" t="s">
+        <v>132</v>
+      </c>
+      <c r="E44" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>132</v>
+      </c>
+      <c r="B45" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45" t="s">
+        <v>132</v>
+      </c>
+      <c r="E45" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>132</v>
+      </c>
+      <c r="B46" t="s">
+        <v>132</v>
+      </c>
+      <c r="C46" t="s">
+        <v>132</v>
+      </c>
+      <c r="D46" t="s">
+        <v>132</v>
+      </c>
+      <c r="E46" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>132</v>
+      </c>
+      <c r="B47" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47" t="s">
+        <v>132</v>
+      </c>
+      <c r="D47" t="s">
+        <v>132</v>
+      </c>
+      <c r="E47" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>132</v>
+      </c>
+      <c r="B48" t="s">
+        <v>132</v>
+      </c>
+      <c r="C48" t="s">
+        <v>132</v>
+      </c>
+      <c r="D48" t="s">
+        <v>132</v>
+      </c>
+      <c r="E48" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>132</v>
+      </c>
+      <c r="B49" t="s">
+        <v>132</v>
+      </c>
+      <c r="C49" t="s">
+        <v>132</v>
+      </c>
+      <c r="D49" t="s">
+        <v>132</v>
+      </c>
+      <c r="E49" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>132</v>
+      </c>
+      <c r="B50" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" t="s">
+        <v>132</v>
+      </c>
+      <c r="D50" t="s">
+        <v>132</v>
+      </c>
+      <c r="E50" t="s">
+        <v>132</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:E4"/>
+    <mergeCell ref="A29:E31"/>
+    <mergeCell ref="A35:E37"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1450,8 +2125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1462,7 +2137,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -1470,15 +2145,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -1486,18 +2161,18 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
STP and agrigation added
</commit_message>
<xml_diff>
--- a/data/documentation.xlsx
+++ b/data/documentation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\packetTracerProject\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holyp\OneDrive\Desktop\univer\packetTracerProject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="IP-plan" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="134">
   <si>
     <t>IP-address</t>
   </si>
@@ -426,6 +426,9 @@
   </si>
   <si>
     <t>FILL</t>
+  </si>
+  <si>
+    <t>FA 0/2 - FA 0/6</t>
   </si>
 </sst>
 </file>
@@ -533,14 +536,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -825,7 +828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A29" sqref="A29:B29"/>
     </sheetView>
   </sheetViews>
@@ -1492,10 +1495,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H50" sqref="H50:I51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1525,27 +1528,27 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1602,7 +1605,7 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>73</v>
+        <v>133</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>28</v>
@@ -1627,33 +1630,33 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4">
+        <v>2.2999999999999998</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4">
@@ -1663,23 +1666,23 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" s="4">
-        <v>3</v>
-      </c>
-      <c r="E14" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4">
+        <v>2.2999999999999998</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D15" s="4">
         <v>3</v>
@@ -1688,464 +1691,490 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="4">
+        <v>3</v>
+      </c>
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="4">
-        <v>3</v>
-      </c>
-      <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="B19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="4">
+        <v>3</v>
+      </c>
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>28</v>
-      </c>
+      <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D20" s="4"/>
-      <c r="E20" s="4" t="s">
-        <v>81</v>
+      <c r="E20" s="4">
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="B21" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="4">
-        <v>101</v>
-      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
+      <c r="A22" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B22" s="4" t="s">
-        <v>77</v>
+        <v>133</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="4">
-        <v>102</v>
-      </c>
-      <c r="E22" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D23" s="4">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="D24" s="4">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
+      <c r="B25" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="4">
+        <v>103</v>
+      </c>
       <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4" t="s">
-        <v>82</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="D26" s="4">
+        <v>104</v>
+      </c>
+      <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D29" s="4">
         <v>101</v>
       </c>
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4" t="s">
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D30" s="4">
         <v>104</v>
       </c>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B34" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C34" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="14"/>
-      <c r="E32" s="15">
+      <c r="D34" s="13"/>
+      <c r="E34" s="14">
         <v>4.5</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="11" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
+      <c r="B35" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C35" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D33" s="14"/>
-      <c r="E33" s="15">
+      <c r="D35" s="13"/>
+      <c r="E35" s="14">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="11" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C36" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="D34" s="14"/>
-      <c r="E34" s="15">
+      <c r="D36" s="13"/>
+      <c r="E36" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B40" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C40" s="11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="11" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C41" s="11" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="11" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C42" s="11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B44" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C44" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>132</v>
-      </c>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="D45" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E45" s="13" t="s">
+      <c r="A45" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E45" s="12" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E46" s="13" t="s">
+      <c r="A46" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E46" s="12" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E47" s="13" t="s">
+      <c r="A47" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E47" s="12" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="B48" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="D48" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E48" s="13" t="s">
+      <c r="A48" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E48" s="12" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E49" s="13" t="s">
+      <c r="A49" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E49" s="12" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="B50" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E50" s="13" t="s">
+      <c r="A50" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E50" s="12" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="B51" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="D51" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E51" s="13" t="s">
+      <c r="A51" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E51" s="12" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
+      <c r="A52" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
+      <c r="A53" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="13"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:E4"/>
-    <mergeCell ref="A29:E31"/>
-    <mergeCell ref="A35:E37"/>
+    <mergeCell ref="A31:E33"/>
+    <mergeCell ref="A37:E39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>